<commit_message>
feat(extracao): Aprimora prompt do LLaVA e remove fallback de OCR
</commit_message>
<xml_diff>
--- a/Planilha/planilha de dados.xlsx
+++ b/Planilha/planilha de dados.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pure\Desktop\projeto2\Planilha\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03830FAF-EA5D-4C97-A8DB-23C76DB10D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t>hash</t>
   </si>
@@ -112,80 +106,116 @@
     <t>valor_total_impostos</t>
   </si>
   <si>
+    <t>6b4ccb05496145fda961038a16b1a2d1</t>
+  </si>
+  <si>
     <t>405a233a317d0adf17b0f4d02beef0e5</t>
   </si>
   <si>
+    <t>nfe.jpg</t>
+  </si>
+  <si>
     <t>WhatsApp Image 2025-08-20 at 20.50.35.jpeg</t>
   </si>
   <si>
-    <t>2025-08-24 16:51:37</t>
-  </si>
-  <si>
-    <t>00016838</t>
-  </si>
-  <si>
-    <t>2018-11-18 00:00:00</t>
-  </si>
-  <si>
-    <t>LUES-8XKJ</t>
-  </si>
-  <si>
-    <t>00.126.717/0001-84</t>
-  </si>
-  <si>
-    <t>CLINICA VALERIO LTDA</t>
-  </si>
-  <si>
-    <t>R PORTO XAVIER 00066</t>
-  </si>
-  <si>
-    <t>TAQUERA</t>
-  </si>
-  <si>
-    <t>08210-170</t>
-  </si>
-  <si>
-    <t>São Paulo</t>
+    <t>2025-09-06 19:42:31</t>
+  </si>
+  <si>
+    <t>2025-09-06 19:43:23</t>
+  </si>
+  <si>
+    <t>0000000012345678</t>
+  </si>
+  <si>
+    <t>000000000000000</t>
+  </si>
+  <si>
+    <t>2023-09-29T12:34:56.789</t>
+  </si>
+  <si>
+    <t>2019-09-30T15:15:16</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>12.345.678/00-00</t>
+  </si>
+  <si>
+    <t>SERVICOS DE ELECTRONICA LTDA.</t>
+  </si>
+  <si>
+    <t>SERVICOS DE CONSULTORIA LTDA.</t>
+  </si>
+  <si>
+    <t>RUA EXAMPLO, 123 - BLOCO A, APARTAMENTO 123</t>
+  </si>
+  <si>
+    <t>RUA JOSÉ DO NACIONAL, 1234 - BLOCO A, APARTAMENTO 501</t>
+  </si>
+  <si>
+    <t>EXAMPLO</t>
+  </si>
+  <si>
+    <t>SANTO ANTÔNIO</t>
+  </si>
+  <si>
+    <t>12345-678</t>
+  </si>
+  <si>
+    <t>89.000-000</t>
+  </si>
+  <si>
+    <t>SAO PAULO</t>
   </si>
   <si>
     <t>SP</t>
   </si>
   <si>
-    <t>2.276.461-5</t>
-  </si>
-  <si>
-    <t>050.972.418-09</t>
-  </si>
-  <si>
-    <t>DIELSON DOS PASSOS MENDES</t>
-  </si>
-  <si>
-    <t>R Salvador do Sul 154, APTO 02 BL 02</t>
-  </si>
-  <si>
-    <t>Vila Progresso (Zona Leste)</t>
-  </si>
-  <si>
-    <t>08240-500</t>
-  </si>
-  <si>
-    <t>dielsonmendes@hotmail.com</t>
-  </si>
-  <si>
-    <t>REFERENTE A SERVIÇOS ODONTOLOGICO DO MESMO</t>
-  </si>
-  <si>
-    <t>04893</t>
-  </si>
-  <si>
-    <t>Odontologia.</t>
+    <t>INSCRIÇÃO MUNICIPAL 1234567890</t>
+  </si>
+  <si>
+    <t>INSCRITA NO MUNICÍPIO DE SAN PEDRO</t>
+  </si>
+  <si>
+    <t>00.000.000-00</t>
+  </si>
+  <si>
+    <t>123.456.789-00</t>
+  </si>
+  <si>
+    <t>NOME DA PERSONA</t>
+  </si>
+  <si>
+    <t>EMPRESA DE COMÉRCIO E SERVICOS LTDA.</t>
+  </si>
+  <si>
+    <t>exemplo@email.com</t>
+  </si>
+  <si>
+    <t>contato@empresa.com.br</t>
+  </si>
+  <si>
+    <t>TROCA DE SERVICO</t>
+  </si>
+  <si>
+    <t>SERVIÇO DE CONSULTORIA</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>99.000-000</t>
+  </si>
+  <si>
+    <t>CONSULTORIA EM MARKETING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,21 +278,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -300,7 +322,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -334,7 +356,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -369,10 +390,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -545,19 +565,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="23" max="23" width="30.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,96 +664,188 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="N2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" t="s">
         <v>44</v>
       </c>
-      <c r="P2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>46</v>
-      </c>
-      <c r="R2" t="s">
-        <v>47</v>
       </c>
       <c r="S2" t="s">
         <v>48</v>
       </c>
       <c r="T2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" t="s">
+        <v>60</v>
+      </c>
+      <c r="X2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z2">
+        <v>60</v>
+      </c>
+      <c r="AA2">
+        <v>50</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>9</v>
+      </c>
+      <c r="AD2">
+        <v>7.34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="U2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
         <v>49</v>
       </c>
-      <c r="W2" t="s">
+      <c r="L3" t="s">
         <v>50</v>
       </c>
-      <c r="X2" t="s">
+      <c r="M3" t="s">
         <v>51</v>
       </c>
-      <c r="Y2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z2">
+      <c r="N3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z3">
+        <v>1500</v>
+      </c>
+      <c r="AA3">
         <v>1200</v>
       </c>
-      <c r="AA2">
-        <v>1200</v>
-      </c>
-      <c r="AB2">
-        <v>0.02</v>
-      </c>
-      <c r="AC2">
-        <v>24</v>
-      </c>
-      <c r="AD2">
-        <v>195.96</v>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>1800</v>
+      </c>
+      <c r="AD3">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Salvando trabalho local antes do merge
</commit_message>
<xml_diff>
--- a/Planilha/planilha de dados.xlsx
+++ b/Planilha/planilha de dados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>hash</t>
   </si>
@@ -40,6 +40,9 @@
     <t>prestador_razao_social</t>
   </si>
   <si>
+    <t>prestador_inscricao_municipal</t>
+  </si>
+  <si>
     <t>prestador_logradouro</t>
   </si>
   <si>
@@ -55,15 +58,15 @@
     <t>prestador_uf</t>
   </si>
   <si>
-    <t>prestador_inscricao_municipal</t>
-  </si>
-  <si>
     <t>tomador_cpf</t>
   </si>
   <si>
     <t>tomador_razao_social</t>
   </si>
   <si>
+    <t>tomador_email</t>
+  </si>
+  <si>
     <t>tomador_logradouro</t>
   </si>
   <si>
@@ -79,9 +82,6 @@
     <t>tomador_uf</t>
   </si>
   <si>
-    <t>tomador_email</t>
-  </si>
-  <si>
     <t>discriminacao_servicos</t>
   </si>
   <si>
@@ -118,22 +118,25 @@
     <t>WhatsApp Image 2025-08-20 at 20.50.35.jpeg</t>
   </si>
   <si>
-    <t>2025-09-06 19:42:31</t>
-  </si>
-  <si>
-    <t>2025-09-06 19:43:23</t>
-  </si>
-  <si>
-    <t>0000000012345678</t>
-  </si>
-  <si>
-    <t>000000000000000</t>
-  </si>
-  <si>
-    <t>2023-09-29T12:34:56.789</t>
-  </si>
-  <si>
-    <t>2019-09-30T15:15:16</t>
+    <t>2025-09-14 14:39:04</t>
+  </si>
+  <si>
+    <t>2025-09-14 14:40:03</t>
+  </si>
+  <si>
+    <t>0001234567890123</t>
+  </si>
+  <si>
+    <t>0000000000000000</t>
+  </si>
+  <si>
+    <t>2023-03-15T12:34:56.789</t>
+  </si>
+  <si>
+    <t>2019-09-30T00:00:00</t>
+  </si>
+  <si>
+    <t>1234567890123456</t>
   </si>
   <si>
     <t>1234567890</t>
@@ -148,67 +151,70 @@
     <t>SERVICOS DE CONSULTORIA LTDA.</t>
   </si>
   <si>
-    <t>RUA EXAMPLO, 123 - BLOCO A, APARTAMENTO 123</t>
-  </si>
-  <si>
-    <t>RUA JOSÉ DO NACIONAL, 1234 - BLOCO A, APARTAMENTO 501</t>
-  </si>
-  <si>
-    <t>EXAMPLO</t>
-  </si>
-  <si>
-    <t>SANTO ANTÔNIO</t>
+    <t>INSCRIÇÃO MUNICIPAL 123456789012345</t>
+  </si>
+  <si>
+    <t>Rua Exemplo, 123 - Bairro Novo, Cidade</t>
+  </si>
+  <si>
+    <t>Rua Exemplo, 123 - Bairro Novo, Cidade, Estado</t>
+  </si>
+  <si>
+    <t>Novos</t>
   </si>
   <si>
     <t>12345-678</t>
   </si>
   <si>
-    <t>89.000-000</t>
-  </si>
-  <si>
-    <t>SAO PAULO</t>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Cidade</t>
   </si>
   <si>
     <t>SP</t>
   </si>
   <si>
-    <t>INSCRIÇÃO MUNICIPAL 1234567890</t>
-  </si>
-  <si>
-    <t>INSCRITA NO MUNICÍPIO DE SAN PEDRO</t>
-  </si>
-  <si>
     <t>00.000.000-00</t>
   </si>
   <si>
-    <t>123.456.789-00</t>
-  </si>
-  <si>
-    <t>NOME DA PERSONA</t>
-  </si>
-  <si>
-    <t>EMPRESA DE COMÉRCIO E SERVICOS LTDA.</t>
-  </si>
-  <si>
-    <t>exemplo@email.com</t>
-  </si>
-  <si>
-    <t>contato@empresa.com.br</t>
+    <t>EMPRESA DE COMÉRCIO ESTÁTICO</t>
+  </si>
+  <si>
+    <t>Nome da Empresa</t>
+  </si>
+  <si>
+    <t>contato@exemplo.com</t>
+  </si>
+  <si>
+    <t>Rua Exemplo, 456 - Bairro Novo, Cidade</t>
+  </si>
+  <si>
+    <t>Rua Exemplo, 234 - Bairro Novo, Cidade, Estado</t>
+  </si>
+  <si>
+    <t>Novo</t>
+  </si>
+  <si>
+    <t>12345-000</t>
   </si>
   <si>
     <t>TROCA DE SERVICO</t>
   </si>
   <si>
-    <t>SERVIÇO DE CONSULTORIA</t>
-  </si>
-  <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>99.000-000</t>
-  </si>
-  <si>
-    <t>CONSULTORIA EM MARKETING</t>
+    <t>SERVICOS DE CONSULTORIA</t>
+  </si>
+  <si>
+    <t>99.999.000-00</t>
+  </si>
+  <si>
+    <t>99.000.000-00</t>
+  </si>
+  <si>
+    <t>SERVIÇO DE TROCA DE ELETRÔNICOS</t>
+  </si>
+  <si>
+    <t>Consultoria em Marketing</t>
   </si>
 </sst>
 </file>
@@ -684,13 +690,13 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
         <v>46</v>
@@ -699,7 +705,7 @@
         <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M2" t="s">
         <v>51</v>
@@ -708,52 +714,52 @@
         <v>52</v>
       </c>
       <c r="O2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" t="s">
         <v>54</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>56</v>
       </c>
-      <c r="Q2" t="s">
-        <v>44</v>
-      </c>
       <c r="R2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="S2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="T2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="U2" t="s">
         <v>51</v>
       </c>
       <c r="V2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="W2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="X2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Y2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="Z2">
-        <v>60</v>
+        <v>600</v>
       </c>
       <c r="AA2">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="AD2">
-        <v>7.34</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -773,22 +779,22 @@
         <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
         <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
       </c>
       <c r="J3" t="s">
         <v>47</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s">
         <v>50</v>
@@ -797,22 +803,22 @@
         <v>51</v>
       </c>
       <c r="N3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" t="s">
         <v>53</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>55</v>
       </c>
-      <c r="P3" t="s">
-        <v>57</v>
-      </c>
       <c r="Q3" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="S3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="T3" t="s">
         <v>50</v>
@@ -821,31 +827,31 @@
         <v>51</v>
       </c>
       <c r="V3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="W3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Y3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Z3">
         <v>1500</v>
       </c>
       <c r="AA3">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="AB3">
         <v>0</v>
       </c>
       <c r="AC3">
-        <v>1800</v>
+        <v>1575</v>
       </c>
       <c r="AD3">
-        <v>250</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(auth): Implementa sistema completo de login e gestão de utilizadores com MySQL
</commit_message>
<xml_diff>
--- a/Planilha/planilha de dados.xlsx
+++ b/Planilha/planilha de dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\projeto2\Planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D486177-1F35-4A5B-A363-812D1C9D0E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBDF5D2-55A1-412F-9ED9-0794AB073F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>